<commit_message>
created way to read from file
</commit_message>
<xml_diff>
--- a/src/main/resources/Movies.xlsx
+++ b/src/main/resources/Movies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Developing\Java\MovieRecommandation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4566D704-B30D-454F-A716-D38F938D1017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FD3812-1939-4F69-ACBD-C5174C628CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,41 +24,76 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Lucian Schipor</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{7A6F8E13-B821-4FEA-9C78-F1C2C6C884C6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucian Schipor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t xml:space="preserve">Title </t>
+    <t xml:space="preserve">Avengers </t>
   </si>
   <si>
-    <t xml:space="preserve">Studio </t>
+    <t xml:space="preserve">Fantasy </t>
   </si>
   <si>
-    <t>Likes</t>
-  </si>
-  <si>
-    <t>dsad</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>sa</t>
-  </si>
-  <si>
-    <t>a</t>
+    <t xml:space="preserve">Marvel </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,8 +116,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,16 +399,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="7" width="16.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,42 +422,15 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="D1" s="1">
+        <v>44107</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>5</v>
+      <c r="E1" s="2">
+        <v>16093323</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>